<commit_message>
push complex query and final edit mock data
</commit_message>
<xml_diff>
--- a/stored_excel/message.xlsx
+++ b/stored_excel/message.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rutth\git\tortoise-app-sql\Stored .xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rutth\git\tortoise-app-sql\stored_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CEAE34-253E-4086-86C8-29B75E9A4690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600BC1A8-9680-422A-BC1C-663BEAD4D551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7E370924-37A2-4CC1-B37B-4E1F6C29CE33}"/>
+    <workbookView xWindow="-36" yWindow="0" windowWidth="10896" windowHeight="12360" xr2:uid="{7E370924-37A2-4CC1-B37B-4E1F6C29CE33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
   <si>
     <t>CHAT001</t>
   </si>
@@ -75,6 +75,159 @@
   </si>
   <si>
     <t>Hi</t>
+  </si>
+  <si>
+    <t>CHAT003</t>
+  </si>
+  <si>
+    <t>C003</t>
+  </si>
+  <si>
+    <t>P005</t>
+  </si>
+  <si>
+    <t>P007</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>You nigga</t>
+  </si>
+  <si>
+    <t>Shutup asian</t>
+  </si>
+  <si>
+    <t>fuck you</t>
+  </si>
+  <si>
+    <t>tell your father to use condom next time</t>
+  </si>
+  <si>
+    <t>CHAT00D</t>
+  </si>
+  <si>
+    <t>C006</t>
+  </si>
+  <si>
+    <t>C007</t>
+  </si>
+  <si>
+    <t>C009</t>
+  </si>
+  <si>
+    <t>asia</t>
+  </si>
+  <si>
+    <t>nigeria country</t>
+  </si>
+  <si>
+    <t>noodle</t>
+  </si>
+  <si>
+    <t>appoint</t>
+  </si>
+  <si>
+    <t>CHAT010</t>
+  </si>
+  <si>
+    <t>CHAT011</t>
+  </si>
+  <si>
+    <t>CHAT012</t>
+  </si>
+  <si>
+    <t>CHAT013</t>
+  </si>
+  <si>
+    <t>CHAT014</t>
+  </si>
+  <si>
+    <t>CHAT015</t>
+  </si>
+  <si>
+    <t>CHAT016</t>
+  </si>
+  <si>
+    <t>CHAT017</t>
+  </si>
+  <si>
+    <t>CHAT018</t>
+  </si>
+  <si>
+    <t>CHAT019</t>
+  </si>
+  <si>
+    <t>P003</t>
+  </si>
+  <si>
+    <t>P001</t>
+  </si>
+  <si>
+    <t>P004</t>
+  </si>
+  <si>
+    <t>shit</t>
+  </si>
+  <si>
+    <t>shite</t>
+  </si>
+  <si>
+    <t>motherfucker</t>
+  </si>
+  <si>
+    <t>fuck dad bad sex</t>
+  </si>
+  <si>
+    <t>nigger</t>
+  </si>
+  <si>
+    <t>black boy</t>
+  </si>
+  <si>
+    <t>no appointment anymore</t>
+  </si>
+  <si>
+    <t>niger</t>
+  </si>
+  <si>
+    <t>fuck smash</t>
+  </si>
+  <si>
+    <t>smash shit</t>
+  </si>
+  <si>
+    <t>bullshit</t>
+  </si>
+  <si>
+    <t>your shithead</t>
+  </si>
+  <si>
+    <t>fuck you too</t>
+  </si>
+  <si>
+    <t>cause you're fucking shite</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>you black nigger shall shutup</t>
+  </si>
+  <si>
+    <t>better soceity please</t>
+  </si>
+  <si>
+    <t>fu ck er</t>
+  </si>
+  <si>
+    <t>hemp n I g g e r</t>
   </si>
 </sst>
 </file>
@@ -439,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8109D7-D560-490E-B649-C842F462CDF1}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,13 +675,466 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44678.440543923614</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44679.440543923614</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44680.440543923614</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44681.440543923614</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44682.440543923614</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44683.440543923614</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44684.440543923614</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44685.440543923614</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44686.440543923614</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44687.440543923614</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44688.440543923614</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44689.440543923614</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44690.440543923614</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44691.440543923614</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44692.440543923614</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44693.440543923614</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44694.440543923614</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44695.440543923614</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44696.440543923614</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44697.440543923614</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44698.440543923614</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44699.440543923614</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44700.440543923614</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44701.440543923614</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44702.440543923614</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44703.440543923614</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44704.440543923614</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44705.440543923614</v>
+      </c>
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="1">
+        <v>44706.440543923614</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44707.440543923614</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44708.440543923614</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="1">
+        <v>44709.440543923614</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="1">
+        <v>44710.440543923614</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>